<commit_message>
cache hit working in the excel model
</commit_message>
<xml_diff>
--- a/CacheModel.xlsx
+++ b/CacheModel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>CACHE</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>INDEX</t>
+  </si>
+  <si>
+    <t>OFFSET</t>
   </si>
 </sst>
 </file>
@@ -386,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:S19"/>
+  <dimension ref="B1:S19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -398,6 +401,23 @@
     <col min="5" max="5" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="N1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1">
+        <v>0</v>
+      </c>
+      <c r="Q1">
+        <v>1</v>
+      </c>
+      <c r="R1">
+        <v>2</v>
+      </c>
+      <c r="S1">
+        <v>3</v>
+      </c>
+    </row>
     <row r="2" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>8</v>
@@ -409,7 +429,23 @@
         <v>0</v>
       </c>
       <c r="O2" t="s">
-        <v>5</v>
+        <v>11</v>
+      </c>
+      <c r="P2" t="str">
+        <f>DEC2BIN(P1,2)</f>
+        <v>00</v>
+      </c>
+      <c r="Q2" t="str">
+        <f t="shared" ref="Q2:S2" si="0">DEC2BIN(Q1,2)</f>
+        <v>01</v>
+      </c>
+      <c r="R2" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="S2" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.2">
@@ -417,11 +453,11 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D3" t="str">
         <f>DEC2BIN(C3,8)</f>
-        <v>00000000</v>
+        <v>00000011</v>
       </c>
       <c r="G3" t="s">
         <v>1</v>
@@ -466,11 +502,11 @@
       </c>
       <c r="C4">
         <f>BIN2DEC(D4)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D4" t="str">
         <f>RIGHT(D3,2)</f>
-        <v>00</v>
+        <v>11</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -489,35 +525,35 @@
         <v>00000000</v>
       </c>
       <c r="K4" t="str">
-        <f t="shared" ref="K4:M19" si="0">DEC2BIN(0,8)</f>
+        <f t="shared" ref="K4:M19" si="1">DEC2BIN(0,8)</f>
         <v>00000000</v>
       </c>
       <c r="L4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="M4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="O4" t="str">
-        <f>DEC2BIN(0,8)</f>
+        <f>DEC2BIN(F4*4,8)</f>
         <v>00000000</v>
       </c>
       <c r="P4" t="str">
-        <f t="shared" ref="O4:S7" si="1">DEC2BIN(0,8)</f>
+        <f t="shared" ref="O4:S7" si="2">DEC2BIN(0,8)</f>
         <v>00000000</v>
       </c>
       <c r="Q4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
       <c r="R4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
       <c r="S4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
     </row>
@@ -546,35 +582,39 @@
         <v>0</v>
       </c>
       <c r="J5" t="str">
-        <f t="shared" ref="J5:J19" si="2">DEC2BIN(0,8)</f>
+        <f t="shared" ref="J5:J19" si="3">DEC2BIN(0,8)</f>
         <v>00000000</v>
       </c>
       <c r="K5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="L5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="M5" t="str">
-        <f t="shared" si="0"/>
-        <v>00000000</v>
+        <f t="shared" si="1"/>
+        <v>00000000</v>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" ref="O5:O7" si="4">DEC2BIN(F5*4,8)</f>
+        <v>00000100</v>
       </c>
       <c r="P5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
       <c r="Q5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
       <c r="R5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
       <c r="S5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
     </row>
@@ -592,35 +632,39 @@
         <v>0</v>
       </c>
       <c r="J6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
       <c r="K6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="L6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="M6" t="str">
-        <f t="shared" si="0"/>
-        <v>00000000</v>
+        <f t="shared" si="1"/>
+        <v>00000000</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" si="4"/>
+        <v>00001000</v>
       </c>
       <c r="P6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
       <c r="Q6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
       <c r="R6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
       <c r="S6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
     </row>
@@ -638,35 +682,39 @@
         <v>0</v>
       </c>
       <c r="J7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
       <c r="K7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="L7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="M7" t="str">
-        <f t="shared" si="0"/>
-        <v>00000000</v>
+        <f t="shared" si="1"/>
+        <v>00000000</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="4"/>
+        <v>00001100</v>
       </c>
       <c r="P7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
       <c r="Q7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
       <c r="R7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
       <c r="S7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
     </row>
@@ -688,15 +736,15 @@
         <v>00000000</v>
       </c>
       <c r="K8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="L8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="M8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
     </row>
@@ -714,19 +762,19 @@
         <v>0</v>
       </c>
       <c r="J9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
       <c r="K9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="L9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="M9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
     </row>
@@ -744,19 +792,19 @@
         <v>0</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
       <c r="K10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="L10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="M10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
     </row>
@@ -774,19 +822,19 @@
         <v>0</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="L11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="M11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
     </row>
@@ -804,19 +852,19 @@
         <v>0</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
       <c r="K12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="L12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="M12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
     </row>
@@ -834,19 +882,19 @@
         <v>0</v>
       </c>
       <c r="J13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
       <c r="K13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="L13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="M13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
     </row>
@@ -864,19 +912,19 @@
         <v>0</v>
       </c>
       <c r="J14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
       <c r="K14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="L14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="M14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
     </row>
@@ -894,19 +942,19 @@
         <v>0</v>
       </c>
       <c r="J15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
       <c r="K15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="L15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="M15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
     </row>
@@ -924,19 +972,19 @@
         <v>0</v>
       </c>
       <c r="J16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
       <c r="K16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="L16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="M16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
     </row>
@@ -954,19 +1002,19 @@
         <v>0</v>
       </c>
       <c r="J17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
       <c r="K17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="L17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="M17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
     </row>
@@ -984,19 +1032,19 @@
         <v>0</v>
       </c>
       <c r="J18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
       <c r="K18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="L18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="M18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
     </row>
@@ -1014,19 +1062,19 @@
         <v>0</v>
       </c>
       <c r="J19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
       <c r="K19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="L19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="M19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
started new project in VS
better understanding of task
using visual studio now because its installed at uni
</commit_message>
<xml_diff>
--- a/CacheModel.xlsx
+++ b/CacheModel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>CACHE</t>
   </si>
@@ -28,9 +28,6 @@
   </si>
   <si>
     <t>TAG</t>
-  </si>
-  <si>
-    <t>TAG (2 bits)</t>
   </si>
   <si>
     <t>MEMORY</t>
@@ -53,25 +50,57 @@
   <si>
     <t>OFFSET</t>
   </si>
+  <si>
+    <t>HIT?</t>
+  </si>
+  <si>
+    <t>MATCH?</t>
+  </si>
+  <si>
+    <t>VALID?</t>
+  </si>
+  <si>
+    <t>TAG (1 bit)</t>
+  </si>
+  <si>
+    <t>TAG_LENGTH</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -86,8 +115,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:S19"/>
+  <dimension ref="B1:S35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -402,8 +437,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
       <c r="N1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P1">
         <v>0</v>
@@ -420,7 +461,7 @@
     </row>
     <row r="2" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>4</v>
@@ -429,7 +470,7 @@
         <v>0</v>
       </c>
       <c r="O2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P2" t="str">
         <f>DEC2BIN(P1,2)</f>
@@ -450,7 +491,7 @@
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -465,59 +506,59 @@
       <c r="H3" t="s">
         <v>2</v>
       </c>
-      <c r="I3" t="s">
-        <v>4</v>
+      <c r="I3" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="J3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" t="s">
         <v>6</v>
       </c>
-      <c r="K3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L3" t="s">
-        <v>6</v>
-      </c>
-      <c r="M3" t="s">
-        <v>6</v>
-      </c>
-      <c r="O3" t="s">
-        <v>7</v>
-      </c>
       <c r="P3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <f>BIN2DEC(D4)</f>
-        <v>3</v>
-      </c>
-      <c r="D4" t="str">
-        <f>RIGHT(D3,2)</f>
-        <v>11</v>
-      </c>
-      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="str">
+        <f>RIGHT(D3,C1)</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="3">
         <v>0</v>
       </c>
       <c r="J4" t="str">
@@ -541,7 +582,7 @@
         <v>00000000</v>
       </c>
       <c r="P4" t="str">
-        <f t="shared" ref="O4:S7" si="2">DEC2BIN(0,8)</f>
+        <f t="shared" ref="P4:S19" si="2">DEC2BIN(0,8)</f>
         <v>00000000</v>
       </c>
       <c r="Q4" t="str">
@@ -558,27 +599,27 @@
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1">
         <f>BIN2DEC(D5)</f>
-        <v>0</v>
-      </c>
-      <c r="D5" t="str">
-        <f>MID(D3,3,4)</f>
-        <v>0000</v>
-      </c>
-      <c r="F5">
         <v>1</v>
       </c>
+      <c r="D5" s="1" t="str">
+        <f>MID(D3,4,C2)</f>
+        <v>0001</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="3">
         <v>0</v>
       </c>
       <c r="J5" t="str">
@@ -598,7 +639,7 @@
         <v>00000000</v>
       </c>
       <c r="O5" t="str">
-        <f t="shared" ref="O5:O7" si="4">DEC2BIN(F5*4,8)</f>
+        <f t="shared" ref="O5:O35" si="4">DEC2BIN(F5*4,8)</f>
         <v>00000100</v>
       </c>
       <c r="P5" t="str">
@@ -619,7 +660,7 @@
       </c>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="F6">
+      <c r="F6" s="2">
         <v>2</v>
       </c>
       <c r="G6">
@@ -628,7 +669,7 @@
       <c r="H6">
         <v>0</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="3">
         <v>0</v>
       </c>
       <c r="J6" t="str">
@@ -669,7 +710,14 @@
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="F7">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="b">
+        <f>IF(VLOOKUP(C5,F4:I19,4)=C4,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
         <v>3</v>
       </c>
       <c r="G7">
@@ -678,7 +726,7 @@
       <c r="H7">
         <v>0</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="3">
         <v>0</v>
       </c>
       <c r="J7" t="str">
@@ -719,7 +767,14 @@
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="F8">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="b">
+        <f>IF(VLOOKUP(C5,F4:I19,2)=1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
         <v>4</v>
       </c>
       <c r="G8">
@@ -728,7 +783,7 @@
       <c r="H8">
         <v>0</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="3">
         <v>0</v>
       </c>
       <c r="J8" t="str">
@@ -747,9 +802,36 @@
         <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
+      <c r="O8" t="str">
+        <f t="shared" si="4"/>
+        <v>00010000</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Q8" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="R8" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="S8" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="F9">
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="b">
+        <f>AND(C7,C8)</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
         <v>5</v>
       </c>
       <c r="G9">
@@ -758,7 +840,7 @@
       <c r="H9">
         <v>0</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="3">
         <v>0</v>
       </c>
       <c r="J9" t="str">
@@ -777,9 +859,29 @@
         <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
+      <c r="O9" t="str">
+        <f t="shared" si="4"/>
+        <v>00010100</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Q9" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="R9" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="S9" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="F10">
+      <c r="F10" s="2">
         <v>6</v>
       </c>
       <c r="G10">
@@ -788,7 +890,7 @@
       <c r="H10">
         <v>0</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="3">
         <v>0</v>
       </c>
       <c r="J10" t="str">
@@ -807,9 +909,29 @@
         <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
+      <c r="O10" t="str">
+        <f t="shared" si="4"/>
+        <v>00011000</v>
+      </c>
+      <c r="P10" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Q10" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="R10" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="S10" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="F11">
+      <c r="F11" s="2">
         <v>7</v>
       </c>
       <c r="G11">
@@ -818,7 +940,7 @@
       <c r="H11">
         <v>0</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="3">
         <v>0</v>
       </c>
       <c r="J11" t="str">
@@ -837,9 +959,29 @@
         <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
+      <c r="O11" t="str">
+        <f t="shared" si="4"/>
+        <v>00011100</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Q11" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="R11" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="S11" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="F12">
+      <c r="F12" s="2">
         <v>8</v>
       </c>
       <c r="G12">
@@ -848,7 +990,7 @@
       <c r="H12">
         <v>0</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="3">
         <v>0</v>
       </c>
       <c r="J12" t="str">
@@ -867,9 +1009,29 @@
         <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
+      <c r="O12" t="str">
+        <f t="shared" si="4"/>
+        <v>00100000</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Q12" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="R12" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="S12" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="F13">
+      <c r="F13" s="2">
         <v>9</v>
       </c>
       <c r="G13">
@@ -878,7 +1040,7 @@
       <c r="H13">
         <v>0</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="3">
         <v>0</v>
       </c>
       <c r="J13" t="str">
@@ -897,9 +1059,29 @@
         <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
+      <c r="O13" t="str">
+        <f t="shared" si="4"/>
+        <v>00100100</v>
+      </c>
+      <c r="P13" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Q13" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="R13" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="S13" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="F14">
+      <c r="F14" s="2">
         <v>10</v>
       </c>
       <c r="G14">
@@ -908,7 +1090,7 @@
       <c r="H14">
         <v>0</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="3">
         <v>0</v>
       </c>
       <c r="J14" t="str">
@@ -927,9 +1109,29 @@
         <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
+      <c r="O14" t="str">
+        <f t="shared" si="4"/>
+        <v>00101000</v>
+      </c>
+      <c r="P14" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Q14" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="R14" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="S14" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="F15">
+      <c r="F15" s="2">
         <v>11</v>
       </c>
       <c r="G15">
@@ -938,7 +1140,7 @@
       <c r="H15">
         <v>0</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="3">
         <v>0</v>
       </c>
       <c r="J15" t="str">
@@ -957,9 +1159,29 @@
         <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
+      <c r="O15" t="str">
+        <f t="shared" si="4"/>
+        <v>00101100</v>
+      </c>
+      <c r="P15" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Q15" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="R15" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="S15" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="F16">
+      <c r="F16" s="2">
         <v>12</v>
       </c>
       <c r="G16">
@@ -968,7 +1190,7 @@
       <c r="H16">
         <v>0</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="3">
         <v>0</v>
       </c>
       <c r="J16" t="str">
@@ -987,9 +1209,29 @@
         <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
-    </row>
-    <row r="17" spans="6:13" x14ac:dyDescent="0.2">
-      <c r="F17">
+      <c r="O16" t="str">
+        <f t="shared" si="4"/>
+        <v>00110000</v>
+      </c>
+      <c r="P16" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Q16" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="R16" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="S16" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="17" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="F17" s="2">
         <v>13</v>
       </c>
       <c r="G17">
@@ -998,7 +1240,7 @@
       <c r="H17">
         <v>0</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="3">
         <v>0</v>
       </c>
       <c r="J17" t="str">
@@ -1017,9 +1259,29 @@
         <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
-    </row>
-    <row r="18" spans="6:13" x14ac:dyDescent="0.2">
-      <c r="F18">
+      <c r="O17" t="str">
+        <f t="shared" si="4"/>
+        <v>00110100</v>
+      </c>
+      <c r="P17" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Q17" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="R17" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="S17" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="18" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="F18" s="2">
         <v>14</v>
       </c>
       <c r="G18">
@@ -1028,7 +1290,7 @@
       <c r="H18">
         <v>0</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="3">
         <v>0</v>
       </c>
       <c r="J18" t="str">
@@ -1047,9 +1309,29 @@
         <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
-    </row>
-    <row r="19" spans="6:13" x14ac:dyDescent="0.2">
-      <c r="F19">
+      <c r="O18" t="str">
+        <f t="shared" si="4"/>
+        <v>00111000</v>
+      </c>
+      <c r="P18" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Q18" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="R18" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="S18" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="19" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="F19" s="2">
         <v>15</v>
       </c>
       <c r="G19">
@@ -1058,7 +1340,7 @@
       <c r="H19">
         <v>0</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="3">
         <v>0</v>
       </c>
       <c r="J19" t="str">
@@ -1077,9 +1359,431 @@
         <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
+      <c r="O19" t="str">
+        <f t="shared" si="4"/>
+        <v>00111100</v>
+      </c>
+      <c r="P19" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Q19" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="R19" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="S19" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="20" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="F20" s="2">
+        <v>16</v>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" si="4"/>
+        <v>01000000</v>
+      </c>
+      <c r="P20" t="str">
+        <f t="shared" ref="P20:S35" si="5">DEC2BIN(0,8)</f>
+        <v>00000000</v>
+      </c>
+      <c r="Q20" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="R20" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="S20" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="21" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="D21" s="4"/>
+      <c r="F21" s="2">
+        <v>17</v>
+      </c>
+      <c r="O21" t="str">
+        <f t="shared" si="4"/>
+        <v>01000100</v>
+      </c>
+      <c r="P21" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="Q21" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="R21" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="S21" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="22" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="F22" s="2">
+        <v>18</v>
+      </c>
+      <c r="O22" t="str">
+        <f t="shared" si="4"/>
+        <v>01001000</v>
+      </c>
+      <c r="P22" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="Q22" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="R22" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="S22" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="23" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="F23" s="2">
+        <v>19</v>
+      </c>
+      <c r="O23" t="str">
+        <f t="shared" si="4"/>
+        <v>01001100</v>
+      </c>
+      <c r="P23" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="Q23" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="R23" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="S23" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="24" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="F24" s="2">
+        <v>20</v>
+      </c>
+      <c r="O24" t="str">
+        <f t="shared" si="4"/>
+        <v>01010000</v>
+      </c>
+      <c r="P24" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="Q24" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="R24" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="S24" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="25" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="F25" s="2">
+        <v>21</v>
+      </c>
+      <c r="O25" t="str">
+        <f t="shared" si="4"/>
+        <v>01010100</v>
+      </c>
+      <c r="P25" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="Q25" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="R25" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="S25" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="26" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="F26" s="2">
+        <v>22</v>
+      </c>
+      <c r="O26" t="str">
+        <f t="shared" si="4"/>
+        <v>01011000</v>
+      </c>
+      <c r="P26" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="Q26" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="R26" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="S26" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="27" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="F27" s="2">
+        <v>23</v>
+      </c>
+      <c r="O27" t="str">
+        <f t="shared" si="4"/>
+        <v>01011100</v>
+      </c>
+      <c r="P27" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="Q27" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="R27" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="S27" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="28" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="F28" s="2">
+        <v>24</v>
+      </c>
+      <c r="O28" t="str">
+        <f t="shared" si="4"/>
+        <v>01100000</v>
+      </c>
+      <c r="P28" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="Q28" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="R28" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="S28" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="29" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="F29" s="2">
+        <v>25</v>
+      </c>
+      <c r="O29" t="str">
+        <f t="shared" si="4"/>
+        <v>01100100</v>
+      </c>
+      <c r="P29" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="Q29" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="R29" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="S29" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="30" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="F30" s="2">
+        <v>26</v>
+      </c>
+      <c r="O30" t="str">
+        <f t="shared" si="4"/>
+        <v>01101000</v>
+      </c>
+      <c r="P30" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="Q30" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="R30" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="S30" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="31" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="F31" s="2">
+        <v>27</v>
+      </c>
+      <c r="O31" t="str">
+        <f t="shared" si="4"/>
+        <v>01101100</v>
+      </c>
+      <c r="P31" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="Q31" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="R31" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="S31" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="32" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="F32" s="2">
+        <v>28</v>
+      </c>
+      <c r="O32" t="str">
+        <f t="shared" si="4"/>
+        <v>01110000</v>
+      </c>
+      <c r="P32" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="Q32" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="R32" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="S32" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="33" spans="6:19" x14ac:dyDescent="0.2">
+      <c r="F33" s="2">
+        <v>29</v>
+      </c>
+      <c r="O33" t="str">
+        <f t="shared" si="4"/>
+        <v>01110100</v>
+      </c>
+      <c r="P33" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="Q33" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="R33" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="S33" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="34" spans="6:19" x14ac:dyDescent="0.2">
+      <c r="F34" s="2">
+        <v>30</v>
+      </c>
+      <c r="O34" t="str">
+        <f t="shared" si="4"/>
+        <v>01111000</v>
+      </c>
+      <c r="P34" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="Q34" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="R34" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="S34" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="35" spans="6:19" x14ac:dyDescent="0.2">
+      <c r="F35" s="2">
+        <v>31</v>
+      </c>
+      <c r="O35" t="str">
+        <f t="shared" si="4"/>
+        <v>01111100</v>
+      </c>
+      <c r="P35" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="Q35" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="R35" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="S35" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>